<commit_message>
Adding test cases for Validate Earn Garget on Profile page, plus wait improvements
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13140" tabRatio="700" activeTab="3"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13140" tabRatio="700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -992,6 +991,9 @@
       </rPr>
       <t xml:space="preserve"> Edit the Description </t>
     </r>
+  </si>
+  <si>
+    <t>Bug!!! Not testable</t>
   </si>
 </sst>
 </file>
@@ -1519,9 +1521,6 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3074,11 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,9 +3083,10 @@
     <col min="2" max="2" width="45.140625" customWidth="1"/>
     <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>188</v>
       </c>
@@ -3116,14 +3113,17 @@
       <c r="D2" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>189</v>
       </c>
@@ -3137,12 +3137,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>190</v>
       </c>
@@ -3156,12 +3156,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>191</v>
       </c>
@@ -3175,12 +3175,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>192</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>200</v>
       </c>
@@ -3319,12 +3319,8 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4156,10 +4152,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Breaking Test Conditions into separate files
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13140" tabRatio="700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22380" windowHeight="9750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="210">
   <si>
     <t>ID</t>
   </si>
@@ -221,60 +221,6 @@
     <t>User is able to enter and edit "Description"</t>
   </si>
   <si>
-    <t>TCSS_001</t>
-  </si>
-  <si>
-    <t>TCSS_002</t>
-  </si>
-  <si>
-    <t>TCSS_003-006</t>
-  </si>
-  <si>
-    <t>TCSS_007</t>
-  </si>
-  <si>
-    <t>TCSS_008</t>
-  </si>
-  <si>
-    <t>TCSS_009</t>
-  </si>
-  <si>
-    <t>TCSS_010</t>
-  </si>
-  <si>
-    <t>TCSS_011</t>
-  </si>
-  <si>
-    <t>TCSS_012</t>
-  </si>
-  <si>
-    <t>TCSS_013</t>
-  </si>
-  <si>
-    <t>TCSS_014</t>
-  </si>
-  <si>
-    <t>TCSS_015</t>
-  </si>
-  <si>
-    <t>TCSS_016</t>
-  </si>
-  <si>
-    <t>TCSS_017</t>
-  </si>
-  <si>
-    <t>TCSS_018-019</t>
-  </si>
-  <si>
-    <t>TCSS_020</t>
-  </si>
-  <si>
-    <t>TCSS_021</t>
-  </si>
-  <si>
-    <t>TCSS_022</t>
-  </si>
-  <si>
     <t>Validate "Manage Listings" on ListingManagement page</t>
   </si>
   <si>
@@ -994,6 +940,78 @@
   </si>
   <si>
     <t>Bug!!! Not testable</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>wait for Renu's code</t>
+  </si>
+  <si>
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>TC_003-006</t>
+  </si>
+  <si>
+    <t>TC_007</t>
+  </si>
+  <si>
+    <t>TC_008</t>
+  </si>
+  <si>
+    <t>TC_009</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>TC_018-019</t>
+  </si>
+  <si>
+    <t>TC_021</t>
+  </si>
+  <si>
+    <t>TC_022</t>
+  </si>
+  <si>
+    <t>TC_023</t>
+  </si>
+  <si>
+    <t>TC_024</t>
+  </si>
+  <si>
+    <t>TC_027</t>
+  </si>
+  <si>
+    <t>TC_028</t>
+  </si>
+  <si>
+    <t>TC_025-26</t>
+  </si>
+  <si>
+    <t>TC_029</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1196,6 +1214,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1519,9 +1538,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1554,12 +1571,12 @@
       <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="24" t="str">
+      <c r="G1" s="25" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1crUJuzOtaxP2fNaX4ipazLL3rvBrlcDSKbTdXBV7oU0","How to run Mars webiste using Docker")</f>
         <v>How to run Mars webiste using Docker</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -1580,7 +1597,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>16</v>
@@ -1591,13 +1608,13 @@
       <c r="D2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1608,13 +1625,13 @@
       <c r="D3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>19</v>
@@ -1625,13 +1642,13 @@
       <c r="D4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>20</v>
@@ -1642,13 +1659,13 @@
       <c r="D5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>21</v>
@@ -1659,13 +1676,13 @@
       <c r="D6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>22</v>
@@ -1676,13 +1693,13 @@
       <c r="D7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>23</v>
@@ -1693,13 +1710,13 @@
       <c r="D8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>24</v>
@@ -1710,13 +1727,13 @@
       <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>67</v>
+        <v>196</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>25</v>
@@ -1730,7 +1747,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>26</v>
@@ -1744,7 +1761,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>27</v>
@@ -1758,7 +1775,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>28</v>
@@ -1772,7 +1789,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>71</v>
+        <v>199</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>29</v>
@@ -1786,7 +1803,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>72</v>
+        <v>200</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>30</v>
@@ -1800,7 +1817,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>73</v>
+        <v>201</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>31</v>
@@ -1814,7 +1831,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>32</v>
@@ -1828,7 +1845,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>75</v>
+        <v>202</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
@@ -1842,7 +1859,7 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>34</v>
@@ -1855,6 +1872,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>204</v>
+      </c>
       <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
@@ -1863,6 +1883,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>205</v>
+      </c>
       <c r="B21" s="7" t="s">
         <v>36</v>
       </c>
@@ -1871,6 +1894,9 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>208</v>
+      </c>
       <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1879,6 +1905,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>206</v>
+      </c>
       <c r="B23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1887,6 +1916,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>207</v>
+      </c>
       <c r="B24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1895,6 +1927,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
+        <v>209</v>
+      </c>
       <c r="B25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1936,6 +1971,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
       <c r="B31" s="7" t="s">
         <v>20</v>
       </c>
@@ -3073,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,10 +3135,13 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3114,18 +3153,21 @@
         <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>56</v>
@@ -3135,16 +3177,22 @@
       </c>
       <c r="D5" t="s">
         <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>50</v>
       </c>
+      <c r="E6" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
@@ -3154,158 +3202,179 @@
       </c>
       <c r="D8" t="s">
         <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>53</v>
       </c>
+      <c r="E9" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>164</v>
+      </c>
+      <c r="E11" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>181</v>
+        <v>163</v>
+      </c>
+      <c r="E12" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
         <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>181</v>
+      </c>
+      <c r="E14" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>200</v>
+        <v>182</v>
+      </c>
+      <c r="E15" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3318,10 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3373,10 +3439,10 @@
       <c r="Z1" s="13"/>
     </row>
     <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="27" t="s">
+      <c r="A2" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3394,10 +3460,10 @@
       <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>9</v>
@@ -3408,13 +3474,13 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="20"/>
@@ -3422,13 +3488,13 @@
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="15" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="20"/>
@@ -3446,10 +3512,10 @@
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -3467,10 +3533,10 @@
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>9</v>
@@ -3481,13 +3547,13 @@
       <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="20"/>
@@ -3495,13 +3561,13 @@
       <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="15" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="20"/>
@@ -3519,10 +3585,10 @@
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -3540,10 +3606,10 @@
       <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>9</v>
@@ -3554,13 +3620,13 @@
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="15" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="20"/>
@@ -3568,13 +3634,13 @@
       <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="15" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="20"/>
@@ -3592,10 +3658,10 @@
       <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="A17" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -3613,10 +3679,10 @@
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>9</v>
@@ -3627,13 +3693,13 @@
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="15" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="20"/>
@@ -3641,13 +3707,13 @@
       <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="15" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="20"/>
@@ -3665,10 +3731,10 @@
       <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -3686,10 +3752,10 @@
       <c r="H22" s="20"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>9</v>
@@ -3700,13 +3766,13 @@
       <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="15" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="20"/>
@@ -3714,13 +3780,13 @@
       <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="15" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="20"/>
@@ -3738,10 +3804,10 @@
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="27" t="s">
+      <c r="A27" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="28" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -3759,10 +3825,10 @@
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>9</v>
@@ -3773,13 +3839,13 @@
       <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="15" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="20"/>
@@ -3787,13 +3853,13 @@
       <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="15" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="20"/>
@@ -3811,11 +3877,11 @@
       <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>182</v>
+      <c r="A32" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>164</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>8</v>
@@ -3832,10 +3898,10 @@
       <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>9</v>
@@ -3846,13 +3912,13 @@
       <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="15" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="20"/>
@@ -3860,13 +3926,13 @@
       <c r="H34" s="20"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="15" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="20"/>
@@ -3884,11 +3950,11 @@
       <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>181</v>
+      <c r="A37" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>163</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>8</v>
@@ -3905,10 +3971,10 @@
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>9</v>
@@ -3919,13 +3985,13 @@
       <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="15" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="20"/>
@@ -3933,13 +3999,13 @@
       <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="15" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="20"/>
@@ -3957,11 +4023,11 @@
       <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>199</v>
+      <c r="A42" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>181</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>8</v>
@@ -3978,10 +4044,10 @@
       <c r="H42" s="20"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>9</v>
@@ -3992,13 +4058,13 @@
       <c r="H43" s="20"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="15" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="20"/>
@@ -4006,13 +4072,13 @@
       <c r="H44" s="20"/>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="15" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="20"/>
@@ -4023,10 +4089,10 @@
       <c r="A46" s="21"/>
       <c r="B46" s="22"/>
       <c r="C46" s="15" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="20"/>
@@ -4044,11 +4110,11 @@
       <c r="H47" s="20"/>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B48" s="27" t="s">
-        <v>200</v>
+      <c r="A48" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>182</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>8</v>
@@ -4065,10 +4131,10 @@
       <c r="H48" s="20"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D49" s="16" t="s">
         <v>9</v>
@@ -4079,13 +4145,13 @@
       <c r="H49" s="20"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="15" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="20"/>
@@ -4093,13 +4159,13 @@
       <c r="H50" s="20"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="15" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="20"/>
@@ -4107,13 +4173,13 @@
       <c r="H51" s="20"/>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="15" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="20"/>
@@ -4152,9 +4218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4163,57 +4227,57 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E15" t="str">
         <f>CONCATENATE(A15, " - ", B17)</f>
@@ -4222,32 +4286,32 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E22" t="str">
         <f>CONCATENATE(A22, " - ", B23)</f>
@@ -4256,32 +4320,32 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E29" t="str">
         <f>CONCATENATE(A29, " - ", B31)</f>
@@ -4290,32 +4354,32 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E36" t="str">
         <f>CONCATENATE(A36, " - ", B40)</f>
@@ -4324,27 +4388,27 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E42" t="str">
         <f>CONCATENATE(A42, " - ", B44)</f>
@@ -4353,27 +4417,27 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E48" t="str">
         <f>CONCATENATE(A48, " - ", B52)</f>
@@ -4382,37 +4446,37 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E56" t="str">
         <f>CONCATENATE(A56, " - ", B57)</f>
@@ -4421,37 +4485,37 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E64" t="str">
         <f>CONCATENATE(A64, " - ", B68)</f>
@@ -4460,32 +4524,32 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding test cases: Validation for Delete ListManagement and Search Skills page
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,20 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22380" windowHeight="9750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
     <sheet name="Test Conditions" sheetId="1" r:id="rId2"/>
     <sheet name="Test Cases" sheetId="2" r:id="rId3"/>
-    <sheet name="temporary sheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -251,174 +250,12 @@
     <t>User is able to search by "All Categories"</t>
   </si>
   <si>
-    <t>Categories:</t>
-  </si>
-  <si>
-    <t>Graphics &amp; Design</t>
-  </si>
-  <si>
-    <t>Digital Marketing</t>
-  </si>
-  <si>
-    <t>Writing &amp; Translation</t>
-  </si>
-  <si>
-    <t>Video &amp; Animation</t>
-  </si>
-  <si>
-    <t>Music &amp; Audio</t>
-  </si>
-  <si>
-    <t>Programming &amp; Tech</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Fun &amp; Lifestyle</t>
-  </si>
-  <si>
-    <t>Logo Design</t>
-  </si>
-  <si>
-    <t>Book &amp; Album covers</t>
-  </si>
-  <si>
-    <t>Flyers &amp; Brochures</t>
-  </si>
-  <si>
-    <t>Web &amp; Mobile Design</t>
-  </si>
-  <si>
-    <t>Search &amp; Display Marketing</t>
-  </si>
-  <si>
-    <t>Social Media Marketing</t>
-  </si>
-  <si>
-    <t>Content Marketing</t>
-  </si>
-  <si>
-    <t>Video Marketing</t>
-  </si>
-  <si>
-    <t>Email Marketing</t>
-  </si>
-  <si>
-    <t>Resumes &amp; Cover Letters</t>
-  </si>
-  <si>
-    <t>Proof Reading &amp; Editing</t>
-  </si>
-  <si>
-    <t>Translation</t>
-  </si>
-  <si>
-    <t>Creative Writing</t>
-  </si>
-  <si>
-    <t>Business Copywriting</t>
-  </si>
-  <si>
-    <t>Promotional Videos</t>
-  </si>
-  <si>
-    <t>Editing &amp; Post Production</t>
-  </si>
-  <si>
-    <t>Lyric &amp; Music Videos</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Mixing &amp; Mastering</t>
-  </si>
-  <si>
-    <t>Voice Over</t>
-  </si>
-  <si>
-    <t>Song Writers &amp; Composers</t>
-  </si>
-  <si>
-    <t>WordPress</t>
-  </si>
-  <si>
-    <t>Web &amp; Mobile App</t>
-  </si>
-  <si>
-    <t>Data Analysis &amp; Reports</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Business Tips</t>
-  </si>
-  <si>
-    <t>Presentations</t>
-  </si>
-  <si>
-    <t>Market Advice</t>
-  </si>
-  <si>
-    <t>Legal Consulting</t>
-  </si>
-  <si>
-    <t>Financial Consulting</t>
-  </si>
-  <si>
-    <t>Online Lessons</t>
-  </si>
-  <si>
-    <t>Relationship Advice</t>
-  </si>
-  <si>
-    <t>Astrology</t>
-  </si>
-  <si>
-    <t>Health, Nutrition &amp; Fitness</t>
-  </si>
-  <si>
-    <t>Gaming</t>
-  </si>
-  <si>
-    <t>All Categories with subcategories:</t>
-  </si>
-  <si>
     <t>Check if the user is able to search by "All Categories"</t>
   </si>
   <si>
     <t>User is able to search by "Sub Categories"</t>
   </si>
   <si>
-    <t>Check if the user is able to search by "Graphics &amp; Design - Book &amp; Album covers" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Digital Marketing - Social Media Marketing" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Writing &amp; Translation - Proof Reading &amp; Editing" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Video &amp; Animation - Other" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Music &amp; Audio - Voice Over" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Programming &amp; Tech - QA" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Business - Business Tips" Sub Category</t>
-  </si>
-  <si>
-    <t>Check if the user is able to search by "Fun &amp; Lifestyle - Health, Nutrition &amp; Fitness" Sub Category</t>
-  </si>
-  <si>
     <t>User is able to search by "Filter"</t>
   </si>
   <si>
@@ -948,9 +785,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>wait for Renu's code</t>
-  </si>
-  <si>
     <t>TC_001</t>
   </si>
   <si>
@@ -1012,13 +846,280 @@
   </si>
   <si>
     <t>TC_029</t>
+  </si>
+  <si>
+    <t>TC_015_02</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on  "Manage Listings"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able view Share Skill listing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on "Delete" button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on "Yes" Button to confirm</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to click on "Delete"</t>
+  </si>
+  <si>
+    <t>User should be able to click on "Yes" and see a "has been deleted" notification</t>
+  </si>
+  <si>
+    <t>TC_018_00</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on  "Search" with blank entry</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able click "Search" and view "All Categories" search results</t>
+  </si>
+  <si>
+    <t>TC_019_00</t>
+  </si>
+  <si>
+    <t>Check if the user is able to search by "Sub Category"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Go to the URL: "http://localhost:5000/Home/Search"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to load search page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on a "Category"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on a "Sub Category"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 6:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on "Search"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to click on a "Sub Category"</t>
+  </si>
+  <si>
+    <t>User should be able to click on a "Category"</t>
+  </si>
+  <si>
+    <t>User should be able to enter a skill on the Search box</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 6:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Enter a skill in the "Search" box</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to see Search results</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Validate "Received Request" on ReceivedRequest page</t>
+  </si>
+  <si>
+    <t>Check if the user is able to "Accept" request</t>
+  </si>
+  <si>
+    <t>Check if the user is able to "Decline" request</t>
+  </si>
+  <si>
+    <t>User is able to accept and decline "Received Requests"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1077,14 +1178,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1159,14 +1252,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,10 +1298,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1228,6 +1315,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1538,604 +1632,624 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="20" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="7"/>
+    <col min="1" max="1" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="12.5703125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="25" t="str">
+      <c r="G1" s="23" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1crUJuzOtaxP2fNaX4ipazLL3rvBrlcDSKbTdXBV7oU0","How to run Mars webiste using Docker")</f>
         <v>How to run Mars webiste using Docker</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="F4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="F9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="F13" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="F16" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="7" t="s">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="7" t="s">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="7" t="s">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="7" t="s">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3107,274 +3221,274 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="84" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="84" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
+      <c r="E2" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="E3" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E5" t="s">
-        <v>187</v>
+      <c r="E5" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+      <c r="D6" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
-        <v>187</v>
+      <c r="E6" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
-        <v>187</v>
+      <c r="E8" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="D9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E9" t="s">
-        <v>187</v>
+      <c r="E9" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" t="s">
-        <v>187</v>
+      <c r="D11" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" t="s">
-        <v>187</v>
+      <c r="D12" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="E14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="E20" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="E15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>175</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>176</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="E21" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D23" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>121</v>
+      <c r="D25" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>122</v>
+      <c r="A27" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>123</v>
+      <c r="D28" s="30" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>178</v>
-      </c>
-      <c r="B31" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>129</v>
+      <c r="D29" s="30" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3385,1175 +3499,1058 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z52"/>
+  <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="13.85546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18" t="str">
+      <c r="E2" s="16" t="str">
         <f>CONCATENATE(A2,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B2,"""",""))," ",""), "()")</f>
         <v>TC_003_01_CheckIfTheUserIsAbleToSelectTheCountry()</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="18" t="str">
+      <c r="E7" s="16" t="str">
         <f>CONCATENATE(A7,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B7,"""",""))," ",""), "()")</f>
         <v>TC_003_02_CheckIfTheUserIsAbleToEditTheCountry()</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="18" t="str">
+      <c r="E12" s="16" t="str">
         <f>CONCATENATE(A12,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B12,"""",""))," ",""), "()")</f>
         <v>TC_004_01_CheckIfTheUserIsAbleToSelectTheAvailability()</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="28" t="s">
+      <c r="A17" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="18" t="str">
+      <c r="E17" s="16" t="str">
         <f>CONCATENATE(A17,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B17,"""",""))," ",""), "()")</f>
         <v>TC_004_02_CheckIfTheUserIsAbleToEditTheAvailability()</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="16" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="A22" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="18" t="str">
+      <c r="E22" s="16" t="str">
         <f>CONCATENATE(A22,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B22,"""",""))," ",""), "()")</f>
         <v>TC_005_01_CheckIfTheUserIsAbleToSelectTheHours()</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D23" s="16" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="18" t="str">
+      <c r="E27" s="16" t="str">
         <f>CONCATENATE(A27,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B27,"""",""))," ",""), "()")</f>
         <v>TC_005_02_CheckIfTheUserIsAbleToEditTheHours()</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="16"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="C32" s="15" t="s">
+      <c r="A32" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="18" t="str">
+      <c r="E32" s="16" t="str">
         <f>CONCATENATE(A32,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B32,"""",""))," ",""), "()")</f>
         <v>TC_006_01_CheckIfTheUserIsAbleToSelectTheEarnTarget()</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D33" s="16" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="A37" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="18" t="str">
+      <c r="E37" s="16" t="str">
         <f>CONCATENATE(A37,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B37,"""",""))," ",""), "()")</f>
         <v>TC_006_02_CheckIfTheUserIsAbleToEditTheEarnTarget()</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" s="16" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="A42" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="18" t="str">
+      <c r="E42" s="16" t="str">
         <f>CONCATENATE(A42,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B42,"""",""))," ",""), "()")</f>
         <v>TC_011_01_CheckIfTheUserIsAbleToEnterDescripriton()</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D43" s="16" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="16"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E46" s="18"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="16"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" s="15" t="s">
+      <c r="A48" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="18" t="str">
+      <c r="E48" s="16" t="str">
         <f>CONCATENATE(A48,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B48,"""",""))," ",""), "()")</f>
         <v>TC_011_02_CheckIfTheUserIsAbleToEditDescription()</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D49" s="16" t="s">
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="15" t="s">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="16"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+    </row>
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="16"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="16"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="16" t="str">
+        <f>CONCATENATE(A54,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B54,"""",""))," ",""), "()")</f>
+        <v>TC_015_02_CheckIfTheUserIsAbleToDeleteListing()</v>
+      </c>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="25"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="16"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="25"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="16"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="25"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="16"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="25"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D50" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-    </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D51" s="16" t="s">
+      <c r="D58" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E51" s="18"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-    </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="16" t="str">
+        <f>CONCATENATE(A60,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B60,"""",""))," ",""), "()")</f>
+        <v>TC_018_00_CheckIfTheUserIsAbleToSearchByAllCategories()</v>
+      </c>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="25"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="16"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="25"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="16" t="str">
+        <f>CONCATENATE(A64,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B64,"""",""))," ",""), "()")</f>
+        <v>TC_019_00_CheckIfTheUserIsAbleToSearchBySubCategory()</v>
+      </c>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="16"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E66" s="16"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="25"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E67" s="16"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="25"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E68" s="16"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C69" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C70" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>176</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
+  <mergeCells count="26">
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="B48:B52"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" t="str">
-        <f>CONCATENATE(A15, " - ", B17)</f>
-        <v>Graphics &amp; Design - Book &amp; Album covers</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" t="str">
-        <f>CONCATENATE(A22, " - ", B23)</f>
-        <v>Digital Marketing - Social Media Marketing</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" t="str">
-        <f>CONCATENATE(A29, " - ", B31)</f>
-        <v>Writing &amp; Translation - Proof Reading &amp; Editing</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="str">
-        <f>CONCATENATE(A36, " - ", B40)</f>
-        <v>Video &amp; Animation - Other</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" t="str">
-        <f>CONCATENATE(A42, " - ", B44)</f>
-        <v>Music &amp; Audio - Voice Over</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>75</v>
-      </c>
-      <c r="E48" t="str">
-        <f>CONCATENATE(A48, " - ", B52)</f>
-        <v>Programming &amp; Tech - QA</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" t="str">
-        <f>CONCATENATE(A56, " - ", B57)</f>
-        <v>Business - Business Tips</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>77</v>
-      </c>
-      <c r="E64" t="str">
-        <f>CONCATENATE(A64, " - ", B68)</f>
-        <v>Fun &amp; Lifestyle - Health, Nutrition &amp; Fitness</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test cases: Validate Received Request on ReceivedRequest page
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -1113,6 +1114,64 @@
   </si>
   <si>
     <t>User is able to accept and decline "Received Requests"</t>
+  </si>
+  <si>
+    <t>TC_016_01</t>
+  </si>
+  <si>
+    <t>TC_016_02</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on "Manage Requests"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to load "Manage Requests page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on a "Accept" on a received request</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able to click on a "Accept" and see a "Service has been updated" notification</t>
   </si>
 </sst>
 </file>
@@ -1302,6 +1361,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1310,18 +1376,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1635,6 +1694,9 @@
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
+    <sheetView topLeftCell="A10" workbookViewId="1">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1667,12 +1729,12 @@
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="23" t="str">
+      <c r="G1" s="26" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1crUJuzOtaxP2fNaX4ipazLL3rvBrlcDSKbTdXBV7oU0","How to run Mars webiste using Docker")</f>
         <v>How to run Mars webiste using Docker</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1704,9 +1766,9 @@
       <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1721,9 +1783,9 @@
       <c r="D3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1741,9 +1803,9 @@
       <c r="F4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1758,9 +1820,9 @@
       <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1775,9 +1837,9 @@
       <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1792,9 +1854,9 @@
       <c r="D7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -1809,9 +1871,9 @@
       <c r="D8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1829,9 +1891,9 @@
       <c r="F9" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -3223,18 +3285,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+    <sheetView topLeftCell="A22" workbookViewId="1">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="84" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="30"/>
+    <col min="1" max="1" width="13.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="84" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3254,240 +3319,240 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="28" t="s">
+    <row r="3" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="25" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="25" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="25" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="25" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3499,10 +3564,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z70"/>
+  <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="1">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,10 +3623,10 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -3576,8 +3644,8 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="13" t="s">
         <v>126</v>
       </c>
@@ -3590,8 +3658,8 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="13" t="s">
         <v>77</v>
       </c>
@@ -3604,8 +3672,8 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="13" t="s">
         <v>79</v>
       </c>
@@ -3628,10 +3696,10 @@
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="30" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -3649,8 +3717,8 @@
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="13" t="s">
         <v>126</v>
       </c>
@@ -3663,8 +3731,8 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
@@ -3677,8 +3745,8 @@
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="13" t="s">
         <v>82</v>
       </c>
@@ -3701,10 +3769,10 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="30" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -3722,8 +3790,8 @@
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="13" t="s">
         <v>126</v>
       </c>
@@ -3736,8 +3804,8 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
@@ -3750,8 +3818,8 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="13" t="s">
         <v>87</v>
       </c>
@@ -3774,10 +3842,10 @@
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="30" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -3795,8 +3863,8 @@
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="13" t="s">
         <v>126</v>
       </c>
@@ -3809,8 +3877,8 @@
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="13" t="s">
         <v>85</v>
       </c>
@@ -3823,8 +3891,8 @@
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="13" t="s">
         <v>90</v>
       </c>
@@ -3847,10 +3915,10 @@
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -3868,8 +3936,8 @@
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="13" t="s">
         <v>126</v>
       </c>
@@ -3882,8 +3950,8 @@
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="13" t="s">
         <v>93</v>
       </c>
@@ -3896,8 +3964,8 @@
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="13" t="s">
         <v>95</v>
       </c>
@@ -3920,10 +3988,10 @@
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="30" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -3941,8 +4009,8 @@
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="13" t="s">
         <v>126</v>
       </c>
@@ -3955,8 +4023,8 @@
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
@@ -3969,8 +4037,8 @@
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="13" t="s">
         <v>95</v>
       </c>
@@ -3993,10 +4061,10 @@
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="30" t="s">
         <v>110</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4014,8 +4082,8 @@
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="13" t="s">
         <v>126</v>
       </c>
@@ -4028,8 +4096,8 @@
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="13" t="s">
         <v>113</v>
       </c>
@@ -4042,8 +4110,8 @@
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="13" t="s">
         <v>112</v>
       </c>
@@ -4066,10 +4134,10 @@
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="30" t="s">
         <v>109</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -4087,8 +4155,8 @@
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="13" t="s">
         <v>126</v>
       </c>
@@ -4101,8 +4169,8 @@
       <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="13" t="s">
         <v>113</v>
       </c>
@@ -4115,8 +4183,8 @@
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="13" t="s">
         <v>112</v>
       </c>
@@ -4139,10 +4207,10 @@
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="30" t="s">
         <v>127</v>
       </c>
       <c r="C42" s="13" t="s">
@@ -4160,8 +4228,8 @@
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="13" t="s">
         <v>126</v>
       </c>
@@ -4174,8 +4242,8 @@
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="13" t="s">
         <v>129</v>
       </c>
@@ -4188,8 +4256,8 @@
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="13" t="s">
         <v>101</v>
       </c>
@@ -4226,10 +4294,10 @@
       <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="30" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="13" t="s">
@@ -4247,8 +4315,8 @@
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="13" t="s">
         <v>126</v>
       </c>
@@ -4261,8 +4329,8 @@
       <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="13" t="s">
         <v>105</v>
       </c>
@@ -4275,8 +4343,8 @@
       <c r="H50" s="18"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="13" t="s">
         <v>130</v>
       </c>
@@ -4289,8 +4357,8 @@
       <c r="H51" s="18"/>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="26"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="13" t="s">
         <v>103</v>
       </c>
@@ -4303,10 +4371,10 @@
       <c r="H52" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="30" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="13" t="s">
@@ -4324,8 +4392,8 @@
       <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
-      <c r="B55" s="26"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="13" t="s">
         <v>126</v>
       </c>
@@ -4338,8 +4406,8 @@
       <c r="H55" s="18"/>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="26"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="13" t="s">
         <v>156</v>
       </c>
@@ -4352,8 +4420,8 @@
       <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="26"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="30"/>
       <c r="C57" s="13" t="s">
         <v>158</v>
       </c>
@@ -4366,8 +4434,8 @@
       <c r="H57" s="18"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
-      <c r="B58" s="26"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="13" t="s">
         <v>159</v>
       </c>
@@ -4380,11 +4448,11 @@
       <c r="H58" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B60" s="26" t="s">
-        <v>69</v>
+      <c r="A60" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>181</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>8</v>
@@ -4394,15 +4462,15 @@
       </c>
       <c r="E60" s="16" t="str">
         <f>CONCATENATE(A60,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B60,"""",""))," ",""), "()")</f>
-        <v>TC_018_00_CheckIfTheUserIsAbleToSearchByAllCategories()</v>
+        <v>TC_016_01_CheckIfTheUserIsAbleToAcceptRequest()</v>
       </c>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
       <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
-      <c r="B61" s="26"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="29"/>
       <c r="C61" s="13" t="s">
         <v>126</v>
       </c>
@@ -4415,140 +4483,274 @@
       <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
-      <c r="B62" s="26"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="29"/>
       <c r="C62" s="13" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="E62" s="16"/>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
       <c r="H62" s="18"/>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="B64" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="13" t="s">
+    <row r="63" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="28"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E63" s="16"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D65" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E64" s="16" t="str">
-        <f>CONCATENATE(A64,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B64,"""",""))," ",""), "()")</f>
-        <v>TC_019_00_CheckIfTheUserIsAbleToSearchBySubCategory()</v>
-      </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-    </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="16"/>
+      <c r="E65" s="16" t="str">
+        <f>CONCATENATE(A65,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B65,"""",""))," ",""), "()")</f>
+        <v>TC_016_02_CheckIfTheUserIsAbleToDeclineRequest()</v>
+      </c>
       <c r="F65" s="18"/>
       <c r="G65" s="18"/>
       <c r="H65" s="18"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
-      <c r="B66" s="26"/>
+      <c r="A66" s="28"/>
+      <c r="B66" s="29"/>
       <c r="C66" s="13" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
       <c r="H66" s="18"/>
     </row>
-    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
-      <c r="B67" s="26"/>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="28"/>
+      <c r="B67" s="29"/>
       <c r="C67" s="13" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E67" s="16"/>
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
       <c r="H67" s="18"/>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
-      <c r="B68" s="26"/>
+    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="28"/>
+      <c r="B68" s="29"/>
       <c r="C68" s="13" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
     </row>
-    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C69" s="13" t="s">
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B70" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="16" t="str">
+        <f>CONCATENATE(A70,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B70,"""",""))," ",""), "()")</f>
+        <v>TC_018_00_CheckIfTheUserIsAbleToSearchByAllCategories()</v>
+      </c>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="28"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="16"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="28"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E72" s="16"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+    </row>
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="16" t="str">
+        <f>CONCATENATE(A74,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B74,"""",""))," ",""), "()")</f>
+        <v>TC_019_00_CheckIfTheUserIsAbleToSearchBySubCategory()</v>
+      </c>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="28"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="16"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="28"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" s="16"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="28"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="16"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="28"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E78" s="16"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+    </row>
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="28"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D79" s="22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C70" s="13" t="s">
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="28"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D80" s="22" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="B48:B52"/>
+  <mergeCells count="30">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A74:A80"/>
+    <mergeCell ref="B74:B80"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test cases: Validate search by Filter on Search Skills page
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="2"/>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="198">
   <si>
     <t>ID</t>
   </si>
@@ -1098,12 +1097,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Validate "Received Request" on ReceivedRequest page</t>
   </si>
   <si>
@@ -1172,6 +1165,96 @@
   </si>
   <si>
     <t>User should be able to click on a "Accept" and see a "Service has been updated" notification</t>
+  </si>
+  <si>
+    <t>TC_020_01</t>
+  </si>
+  <si>
+    <t>User should be able click "Search"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on  "Online"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able click "Online" and see search results</t>
+  </si>
+  <si>
+    <t>TC_020_02</t>
+  </si>
+  <si>
+    <t>TC_020_03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on  "Onsite"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able click "Onsite" and see search results</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Click on  "ShowAll"</t>
+    </r>
+  </si>
+  <si>
+    <t>User should be able click "ShowAll" and see search results</t>
   </si>
 </sst>
 </file>
@@ -1376,10 +1459,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1691,11 +1774,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-    <sheetView topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1968,7 +2048,7 @@
         <v>43</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2016,7 +2096,7 @@
         <v>43</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3285,11 +3365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
-    <sheetView topLeftCell="A22" workbookViewId="1">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3475,24 +3552,24 @@
         <v>144</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3543,7 +3620,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,13 +3641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z80"/>
+  <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="1">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,7 +3700,7 @@
       <c r="A2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -3645,7 +3719,7 @@
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
-      <c r="B3" s="30"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="13" t="s">
         <v>126</v>
       </c>
@@ -3659,7 +3733,7 @@
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
-      <c r="B4" s="30"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="13" t="s">
         <v>77</v>
       </c>
@@ -3673,7 +3747,7 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="13" t="s">
         <v>79</v>
       </c>
@@ -3699,7 +3773,7 @@
       <c r="A7" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -3718,7 +3792,7 @@
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
-      <c r="B8" s="30"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="13" t="s">
         <v>126</v>
       </c>
@@ -3732,7 +3806,7 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="28"/>
-      <c r="B9" s="30"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
@@ -3746,7 +3820,7 @@
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="13" t="s">
         <v>82</v>
       </c>
@@ -3772,7 +3846,7 @@
       <c r="A12" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -3791,7 +3865,7 @@
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
-      <c r="B13" s="30"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="13" t="s">
         <v>126</v>
       </c>
@@ -3805,7 +3879,7 @@
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
-      <c r="B14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
@@ -3819,7 +3893,7 @@
     </row>
     <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
-      <c r="B15" s="30"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="13" t="s">
         <v>87</v>
       </c>
@@ -3845,7 +3919,7 @@
       <c r="A17" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -3864,7 +3938,7 @@
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
-      <c r="B18" s="30"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="13" t="s">
         <v>126</v>
       </c>
@@ -3878,7 +3952,7 @@
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
-      <c r="B19" s="30"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="13" t="s">
         <v>85</v>
       </c>
@@ -3892,7 +3966,7 @@
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
-      <c r="B20" s="30"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="13" t="s">
         <v>90</v>
       </c>
@@ -3918,7 +3992,7 @@
       <c r="A22" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -3937,7 +4011,7 @@
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
-      <c r="B23" s="30"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="13" t="s">
         <v>126</v>
       </c>
@@ -3951,7 +4025,7 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
-      <c r="B24" s="30"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="13" t="s">
         <v>93</v>
       </c>
@@ -3965,7 +4039,7 @@
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
-      <c r="B25" s="30"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="13" t="s">
         <v>95</v>
       </c>
@@ -3988,10 +4062,10 @@
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="13" t="s">
@@ -4009,8 +4083,8 @@
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="13" t="s">
         <v>126</v>
       </c>
@@ -4023,8 +4097,8 @@
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
@@ -4037,8 +4111,8 @@
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="13" t="s">
         <v>95</v>
       </c>
@@ -4061,10 +4135,10 @@
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>110</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4082,8 +4156,8 @@
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="13" t="s">
         <v>126</v>
       </c>
@@ -4096,8 +4170,8 @@
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="13" t="s">
         <v>113</v>
       </c>
@@ -4110,8 +4184,8 @@
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="13" t="s">
         <v>112</v>
       </c>
@@ -4137,7 +4211,7 @@
       <c r="A37" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>109</v>
       </c>
       <c r="C37" s="13" t="s">
@@ -4156,7 +4230,7 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
-      <c r="B38" s="30"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="13" t="s">
         <v>126</v>
       </c>
@@ -4170,7 +4244,7 @@
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="30"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="13" t="s">
         <v>113</v>
       </c>
@@ -4184,7 +4258,7 @@
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
-      <c r="B40" s="30"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="13" t="s">
         <v>112</v>
       </c>
@@ -4210,7 +4284,7 @@
       <c r="A42" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="29" t="s">
         <v>127</v>
       </c>
       <c r="C42" s="13" t="s">
@@ -4229,7 +4303,7 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
-      <c r="B43" s="30"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="13" t="s">
         <v>126</v>
       </c>
@@ -4243,7 +4317,7 @@
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
-      <c r="B44" s="30"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="13" t="s">
         <v>129</v>
       </c>
@@ -4257,7 +4331,7 @@
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
-      <c r="B45" s="30"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="13" t="s">
         <v>101</v>
       </c>
@@ -4297,7 +4371,7 @@
       <c r="A48" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="29" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="13" t="s">
@@ -4316,7 +4390,7 @@
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="30"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="13" t="s">
         <v>126</v>
       </c>
@@ -4330,7 +4404,7 @@
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
-      <c r="B50" s="30"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="13" t="s">
         <v>105</v>
       </c>
@@ -4344,7 +4418,7 @@
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
-      <c r="B51" s="30"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="13" t="s">
         <v>130</v>
       </c>
@@ -4358,7 +4432,7 @@
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
-      <c r="B52" s="30"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="13" t="s">
         <v>103</v>
       </c>
@@ -4374,7 +4448,7 @@
       <c r="A54" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="29" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="13" t="s">
@@ -4393,7 +4467,7 @@
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
-      <c r="B55" s="30"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="13" t="s">
         <v>126</v>
       </c>
@@ -4407,7 +4481,7 @@
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
-      <c r="B56" s="30"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="13" t="s">
         <v>156</v>
       </c>
@@ -4421,7 +4495,7 @@
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
-      <c r="B57" s="30"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="13" t="s">
         <v>158</v>
       </c>
@@ -4435,7 +4509,7 @@
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
-      <c r="B58" s="30"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="13" t="s">
         <v>159</v>
       </c>
@@ -4449,10 +4523,10 @@
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>179</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>8</v>
@@ -4470,7 +4544,7 @@
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
-      <c r="B61" s="29"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="13" t="s">
         <v>126</v>
       </c>
@@ -4484,12 +4558,12 @@
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
-      <c r="B62" s="29"/>
+      <c r="B62" s="30"/>
       <c r="C62" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E62" s="16"/>
       <c r="F62" s="18"/>
@@ -4498,12 +4572,12 @@
     </row>
     <row r="63" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
-      <c r="B63" s="29"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E63" s="16"/>
       <c r="F63" s="18"/>
@@ -4512,10 +4586,10 @@
     </row>
     <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="B65" s="29" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>180</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>8</v>
@@ -4533,7 +4607,7 @@
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="13" t="s">
         <v>126</v>
       </c>
@@ -4547,12 +4621,12 @@
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
-      <c r="B67" s="29"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E67" s="16"/>
       <c r="F67" s="18"/>
@@ -4561,12 +4635,12 @@
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
-      <c r="B68" s="29"/>
+      <c r="B68" s="30"/>
       <c r="C68" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="18"/>
@@ -4577,7 +4651,7 @@
       <c r="A70" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C70" s="13" t="s">
@@ -4596,7 +4670,7 @@
     </row>
     <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="28"/>
-      <c r="B71" s="30"/>
+      <c r="B71" s="29"/>
       <c r="C71" s="13" t="s">
         <v>126</v>
       </c>
@@ -4610,7 +4684,7 @@
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="28"/>
-      <c r="B72" s="30"/>
+      <c r="B72" s="29"/>
       <c r="C72" s="13" t="s">
         <v>163</v>
       </c>
@@ -4626,7 +4700,7 @@
       <c r="A74" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="30" t="s">
         <v>166</v>
       </c>
       <c r="C74" s="13" t="s">
@@ -4645,7 +4719,7 @@
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="28"/>
-      <c r="B75" s="29"/>
+      <c r="B75" s="30"/>
       <c r="C75" s="13" t="s">
         <v>126</v>
       </c>
@@ -4659,7 +4733,7 @@
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="28"/>
-      <c r="B76" s="29"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="13" t="s">
         <v>167</v>
       </c>
@@ -4673,7 +4747,7 @@
     </row>
     <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="28"/>
-      <c r="B77" s="29"/>
+      <c r="B77" s="30"/>
       <c r="C77" s="13" t="s">
         <v>169</v>
       </c>
@@ -4687,7 +4761,7 @@
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
+      <c r="B78" s="30"/>
       <c r="C78" s="13" t="s">
         <v>170</v>
       </c>
@@ -4701,7 +4775,7 @@
     </row>
     <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="28"/>
-      <c r="B79" s="29"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="13" t="s">
         <v>175</v>
       </c>
@@ -4711,7 +4785,7 @@
     </row>
     <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="28"/>
-      <c r="B80" s="29"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="13" t="s">
         <v>171</v>
       </c>
@@ -4719,16 +4793,207 @@
         <v>176</v>
       </c>
     </row>
+    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="16" t="str">
+        <f>CONCATENATE(A82,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B82,"""",""))," ",""), "()")</f>
+        <v>TC_020_01_CheckIfTheUserIsAbleToSearchByOnlineFilter()</v>
+      </c>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="28"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="16"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="28"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E84" s="16"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="28"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E85" s="16"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="87" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="16" t="str">
+        <f>CONCATENATE(A87,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B87,"""",""))," ",""), "()")</f>
+        <v>TC_020_02_CheckIfTheUserIsAbleToSearchByOnsiteFilter()</v>
+      </c>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="28"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="16"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="28"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="16"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="28"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E90" s="16"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B92" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="16" t="str">
+        <f>CONCATENATE(A92,"_",SUBSTITUTE(PROPER(SUBSTITUTE(B92,"""",""))," ",""), "()")</f>
+        <v>TC_020_03_CheckIfTheUserIsAbleToSearchByShowallFilter()</v>
+      </c>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="28"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="16"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="28"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E94" s="16"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+    </row>
+    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="28"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E95" s="16"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
+  <mergeCells count="36">
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
     <mergeCell ref="A70:A72"/>
     <mergeCell ref="B70:B72"/>
     <mergeCell ref="A74:A80"/>
@@ -4739,18 +5004,22 @@
     <mergeCell ref="B60:B63"/>
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding [SetUpFixture], some improvements and file cleanup.
</commit_message>
<xml_diff>
--- a/Mars Test Conditions and Cases .xlsx
+++ b/Mars Test Conditions and Cases .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="5565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -1255,6 +1255,9 @@
   </si>
   <si>
     <t>User should be able click "ShowAll" and see search results</t>
+  </si>
+  <si>
+    <t>User should be able Click on Edit Description</t>
   </si>
 </sst>
 </file>
@@ -1456,13 +1459,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1774,7 +1777,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3366,7 +3369,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,8 +3646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,7 +3700,7 @@
       <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -3718,7 +3721,7 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="29"/>
       <c r="C3" s="13" t="s">
         <v>126</v>
@@ -3732,7 +3735,7 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="29"/>
       <c r="C4" s="13" t="s">
         <v>77</v>
@@ -3746,7 +3749,7 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="29"/>
       <c r="C5" s="13" t="s">
         <v>79</v>
@@ -3770,7 +3773,7 @@
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="29" t="s">
@@ -3791,7 +3794,7 @@
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="29"/>
       <c r="C8" s="13" t="s">
         <v>126</v>
@@ -3805,7 +3808,7 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="29"/>
       <c r="C9" s="13" t="s">
         <v>77</v>
@@ -3819,7 +3822,7 @@
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="29"/>
       <c r="C10" s="13" t="s">
         <v>82</v>
@@ -3843,7 +3846,7 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="30" t="s">
         <v>84</v>
       </c>
       <c r="B12" s="29" t="s">
@@ -3864,7 +3867,7 @@
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="29"/>
       <c r="C13" s="13" t="s">
         <v>126</v>
@@ -3878,7 +3881,7 @@
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="29"/>
       <c r="C14" s="13" t="s">
         <v>85</v>
@@ -3892,7 +3895,7 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="29"/>
       <c r="C15" s="13" t="s">
         <v>87</v>
@@ -3916,7 +3919,7 @@
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="30" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="29" t="s">
@@ -3937,7 +3940,7 @@
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="29"/>
       <c r="C18" s="13" t="s">
         <v>126</v>
@@ -3951,7 +3954,7 @@
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="29"/>
       <c r="C19" s="13" t="s">
         <v>85</v>
@@ -3965,7 +3968,7 @@
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="29"/>
       <c r="C20" s="13" t="s">
         <v>90</v>
@@ -3989,7 +3992,7 @@
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="30" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="29" t="s">
@@ -4010,7 +4013,7 @@
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="29"/>
       <c r="C23" s="13" t="s">
         <v>126</v>
@@ -4024,7 +4027,7 @@
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="29"/>
       <c r="C24" s="13" t="s">
         <v>93</v>
@@ -4038,7 +4041,7 @@
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="29"/>
       <c r="C25" s="13" t="s">
         <v>95</v>
@@ -4062,7 +4065,7 @@
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>97</v>
       </c>
       <c r="B27" s="29" t="s">
@@ -4083,7 +4086,7 @@
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="29"/>
       <c r="C28" s="13" t="s">
         <v>126</v>
@@ -4097,7 +4100,7 @@
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="29"/>
       <c r="C29" s="13" t="s">
         <v>98</v>
@@ -4111,7 +4114,7 @@
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="29"/>
       <c r="C30" s="13" t="s">
         <v>95</v>
@@ -4135,7 +4138,7 @@
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="29" t="s">
@@ -4156,7 +4159,7 @@
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="29"/>
       <c r="C33" s="13" t="s">
         <v>126</v>
@@ -4170,7 +4173,7 @@
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="13" t="s">
         <v>113</v>
@@ -4184,7 +4187,7 @@
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="13" t="s">
         <v>112</v>
@@ -4208,7 +4211,7 @@
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="30" t="s">
         <v>100</v>
       </c>
       <c r="B37" s="29" t="s">
@@ -4229,7 +4232,7 @@
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="29"/>
       <c r="C38" s="13" t="s">
         <v>126</v>
@@ -4243,7 +4246,7 @@
       <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="29"/>
       <c r="C39" s="13" t="s">
         <v>113</v>
@@ -4257,7 +4260,7 @@
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="29"/>
       <c r="C40" s="13" t="s">
         <v>112</v>
@@ -4281,7 +4284,7 @@
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="30" t="s">
         <v>115</v>
       </c>
       <c r="B42" s="29" t="s">
@@ -4302,7 +4305,7 @@
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="29"/>
       <c r="C43" s="13" t="s">
         <v>126</v>
@@ -4316,13 +4319,13 @@
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="29"/>
       <c r="C44" s="13" t="s">
         <v>129</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="18"/>
@@ -4330,7 +4333,7 @@
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="29"/>
       <c r="C45" s="13" t="s">
         <v>101</v>
@@ -4368,7 +4371,7 @@
       <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="30" t="s">
         <v>125</v>
       </c>
       <c r="B48" s="29" t="s">
@@ -4389,7 +4392,7 @@
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="29"/>
       <c r="C49" s="13" t="s">
         <v>126</v>
@@ -4403,7 +4406,7 @@
       <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="29"/>
       <c r="C50" s="13" t="s">
         <v>105</v>
@@ -4417,7 +4420,7 @@
       <c r="H50" s="18"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="29"/>
       <c r="C51" s="13" t="s">
         <v>130</v>
@@ -4431,7 +4434,7 @@
       <c r="H51" s="18"/>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="29"/>
       <c r="C52" s="13" t="s">
         <v>103</v>
@@ -4445,7 +4448,7 @@
       <c r="H52" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="30" t="s">
         <v>155</v>
       </c>
       <c r="B54" s="29" t="s">
@@ -4466,7 +4469,7 @@
       <c r="H54" s="18"/>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="29"/>
       <c r="C55" s="13" t="s">
         <v>126</v>
@@ -4480,7 +4483,7 @@
       <c r="H55" s="18"/>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="29"/>
       <c r="C56" s="13" t="s">
         <v>156</v>
@@ -4494,7 +4497,7 @@
       <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="29"/>
       <c r="C57" s="13" t="s">
         <v>158</v>
@@ -4508,7 +4511,7 @@
       <c r="H57" s="18"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="29"/>
       <c r="C58" s="13" t="s">
         <v>159</v>
@@ -4522,10 +4525,10 @@
       <c r="H58" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="28" t="s">
         <v>179</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -4543,8 +4546,8 @@
       <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
-      <c r="B61" s="30"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="13" t="s">
         <v>126</v>
       </c>
@@ -4557,8 +4560,8 @@
       <c r="H61" s="18"/>
     </row>
     <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="28"/>
-      <c r="B62" s="30"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="13" t="s">
         <v>184</v>
       </c>
@@ -4571,8 +4574,8 @@
       <c r="H62" s="18"/>
     </row>
     <row r="63" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="28"/>
-      <c r="B63" s="30"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="13" t="s">
         <v>186</v>
       </c>
@@ -4585,10 +4588,10 @@
       <c r="H63" s="18"/>
     </row>
     <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="28" t="s">
         <v>180</v>
       </c>
       <c r="C65" s="13" t="s">
@@ -4606,8 +4609,8 @@
       <c r="H65" s="18"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="28"/>
-      <c r="B66" s="30"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="28"/>
       <c r="C66" s="13" t="s">
         <v>126</v>
       </c>
@@ -4620,8 +4623,8 @@
       <c r="H66" s="18"/>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="28"/>
-      <c r="B67" s="30"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="28"/>
       <c r="C67" s="13" t="s">
         <v>184</v>
       </c>
@@ -4634,8 +4637,8 @@
       <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="28"/>
-      <c r="B68" s="30"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="13" t="s">
         <v>186</v>
       </c>
@@ -4648,7 +4651,7 @@
       <c r="H68" s="18"/>
     </row>
     <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="30" t="s">
         <v>162</v>
       </c>
       <c r="B70" s="29" t="s">
@@ -4669,7 +4672,7 @@
       <c r="H70" s="18"/>
     </row>
     <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="28"/>
+      <c r="A71" s="30"/>
       <c r="B71" s="29"/>
       <c r="C71" s="13" t="s">
         <v>126</v>
@@ -4683,7 +4686,7 @@
       <c r="H71" s="18"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
+      <c r="A72" s="30"/>
       <c r="B72" s="29"/>
       <c r="C72" s="13" t="s">
         <v>163</v>
@@ -4697,10 +4700,10 @@
       <c r="H72" s="18"/>
     </row>
     <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
+      <c r="A74" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="28" t="s">
         <v>166</v>
       </c>
       <c r="C74" s="13" t="s">
@@ -4718,8 +4721,8 @@
       <c r="H74" s="18"/>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="28"/>
-      <c r="B75" s="30"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="13" t="s">
         <v>126</v>
       </c>
@@ -4732,8 +4735,8 @@
       <c r="H75" s="18"/>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
-      <c r="B76" s="30"/>
+      <c r="A76" s="30"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="13" t="s">
         <v>167</v>
       </c>
@@ -4746,8 +4749,8 @@
       <c r="H76" s="18"/>
     </row>
     <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="28"/>
-      <c r="B77" s="30"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="28"/>
       <c r="C77" s="13" t="s">
         <v>169</v>
       </c>
@@ -4760,8 +4763,8 @@
       <c r="H77" s="18"/>
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="30"/>
+      <c r="A78" s="30"/>
+      <c r="B78" s="28"/>
       <c r="C78" s="13" t="s">
         <v>170</v>
       </c>
@@ -4774,8 +4777,8 @@
       <c r="H78" s="18"/>
     </row>
     <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="28"/>
-      <c r="B79" s="30"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="28"/>
       <c r="C79" s="13" t="s">
         <v>175</v>
       </c>
@@ -4784,8 +4787,8 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
-      <c r="B80" s="30"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="28"/>
       <c r="C80" s="13" t="s">
         <v>171</v>
       </c>
@@ -4794,7 +4797,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
+      <c r="A82" s="30" t="s">
         <v>188</v>
       </c>
       <c r="B82" s="29" t="s">
@@ -4815,7 +4818,7 @@
       <c r="H82" s="18"/>
     </row>
     <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="28"/>
+      <c r="A83" s="30"/>
       <c r="B83" s="29"/>
       <c r="C83" s="13" t="s">
         <v>126</v>
@@ -4829,7 +4832,7 @@
       <c r="H83" s="18"/>
     </row>
     <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="28"/>
+      <c r="A84" s="30"/>
       <c r="B84" s="29"/>
       <c r="C84" s="13" t="s">
         <v>163</v>
@@ -4843,7 +4846,7 @@
       <c r="H84" s="18"/>
     </row>
     <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
+      <c r="A85" s="30"/>
       <c r="B85" s="29"/>
       <c r="C85" s="13" t="s">
         <v>190</v>
@@ -4857,7 +4860,7 @@
       <c r="H85" s="18"/>
     </row>
     <row r="87" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="30" t="s">
         <v>192</v>
       </c>
       <c r="B87" s="29" t="s">
@@ -4878,7 +4881,7 @@
       <c r="H87" s="18"/>
     </row>
     <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
+      <c r="A88" s="30"/>
       <c r="B88" s="29"/>
       <c r="C88" s="13" t="s">
         <v>126</v>
@@ -4892,7 +4895,7 @@
       <c r="H88" s="18"/>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
+      <c r="A89" s="30"/>
       <c r="B89" s="29"/>
       <c r="C89" s="13" t="s">
         <v>163</v>
@@ -4906,7 +4909,7 @@
       <c r="H89" s="18"/>
     </row>
     <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
+      <c r="A90" s="30"/>
       <c r="B90" s="29"/>
       <c r="C90" s="13" t="s">
         <v>194</v>
@@ -4920,7 +4923,7 @@
       <c r="H90" s="18"/>
     </row>
     <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="30" t="s">
         <v>193</v>
       </c>
       <c r="B92" s="29" t="s">
@@ -4941,7 +4944,7 @@
       <c r="H92" s="18"/>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
+      <c r="A93" s="30"/>
       <c r="B93" s="29"/>
       <c r="C93" s="13" t="s">
         <v>126</v>
@@ -4955,7 +4958,7 @@
       <c r="H93" s="18"/>
     </row>
     <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
+      <c r="A94" s="30"/>
       <c r="B94" s="29"/>
       <c r="C94" s="13" t="s">
         <v>163</v>
@@ -4969,7 +4972,7 @@
       <c r="H94" s="18"/>
     </row>
     <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
+      <c r="A95" s="30"/>
       <c r="B95" s="29"/>
       <c r="C95" s="13" t="s">
         <v>196</v>
@@ -4984,6 +4987,32 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A74:A80"/>
+    <mergeCell ref="B74:B80"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="A54:A58"/>
@@ -4994,32 +5023,6 @@
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A74:A80"/>
-    <mergeCell ref="B74:B80"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="B92:B95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>